<commit_message>
updated parallel exceution for test cases
</commit_message>
<xml_diff>
--- a/resources/SauceDemo_Manual_Test_Cases.xlsx
+++ b/resources/SauceDemo_Manual_Test_Cases.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="205">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -133,13 +133,13 @@
     <t>TS105</t>
   </si>
   <si>
-    <t>Verify the cart prevents checkout when it is empty</t>
+    <t>Verify user can checkout when the cart is empty</t>
   </si>
   <si>
     <t>TS106</t>
   </si>
   <si>
-    <t>Verify the cart is empty when no items are added</t>
+    <t>Verify the cart is empty when no Products are added</t>
   </si>
   <si>
     <t>TS107</t>
@@ -498,9 +498,6 @@
     <t>TC105.1</t>
   </si>
   <si>
-    <t>Verify user can checkout when the cart is empty</t>
-  </si>
-  <si>
     <t>1. Click on 'Cart'. 2. Observe the 'Checkout' button</t>
   </si>
   <si>
@@ -508,9 +505,6 @@
   </si>
   <si>
     <t>TC106.1</t>
-  </si>
-  <si>
-    <t>Verify the cart is empty when no Products are added</t>
   </si>
   <si>
     <t>1. Click on 'Cart'</t>
@@ -733,10 +727,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -770,14 +764,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -793,9 +779,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -810,7 +810,23 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -825,21 +841,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -849,7 +850,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -862,23 +878,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -893,15 +895,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -928,7 +922,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -940,31 +1078,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -976,139 +1102,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1137,21 +1131,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1169,8 +1148,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1179,8 +1160,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1226,159 +1222,157 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1726,8 +1720,8 @@
   <sheetPr/>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>
@@ -2670,8 +2664,8 @@
   <sheetPr/>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -2839,17 +2833,17 @@
         <v>37</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>146</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>77</v>
@@ -2860,23 +2854,23 @@
     </row>
     <row r="7" customFormat="1" spans="1:9">
       <c r="A7" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>149</v>
+        <v>40</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>77</v>
@@ -2887,25 +2881,25 @@
     </row>
     <row r="8" customFormat="1" ht="43.5" spans="1:9">
       <c r="A8" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="G8" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>77</v>
@@ -2916,23 +2910,23 @@
     </row>
     <row r="9" customFormat="1" spans="1:9">
       <c r="A9" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>77</v>
@@ -3007,7 +3001,7 @@
         <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
@@ -3016,16 +3010,16 @@
         <v>47</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>164</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>77</v>
@@ -3039,7 +3033,7 @@
         <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
@@ -3048,16 +3042,16 @@
         <v>49</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>168</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>77</v>
@@ -3071,7 +3065,7 @@
         <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -3080,16 +3074,16 @@
         <v>51</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>172</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>77</v>
@@ -3103,7 +3097,7 @@
         <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
@@ -3112,16 +3106,16 @@
         <v>53</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="H5" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>77</v>
@@ -3135,7 +3129,7 @@
         <v>54</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>8</v>
@@ -3144,16 +3138,16 @@
         <v>55</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>77</v>
@@ -3167,7 +3161,7 @@
         <v>56</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
@@ -3176,16 +3170,16 @@
         <v>57</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>77</v>
@@ -3199,25 +3193,25 @@
         <v>58</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>186</v>
-      </c>
       <c r="H8" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>77</v>
@@ -3231,25 +3225,25 @@
         <v>58</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>190</v>
-      </c>
       <c r="G9" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>77</v>
@@ -3263,25 +3257,25 @@
         <v>58</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>194</v>
-      </c>
       <c r="G10" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>77</v>
@@ -3295,25 +3289,25 @@
         <v>60</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>198</v>
-      </c>
       <c r="G11" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>77</v>
@@ -3327,25 +3321,25 @@
         <v>60</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>202</v>
-      </c>
       <c r="G12" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>77</v>
@@ -3359,25 +3353,25 @@
         <v>62</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>206</v>
-      </c>
       <c r="G13" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>77</v>

</xml_diff>